<commit_message>
Corrected Loading of Generation Data Added Calculation w.o. Heat Seperation
</commit_message>
<xml_diff>
--- a/input/blocks.xlsx
+++ b/input/blocks.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yanni\Documents\09_Job\HiWi\02_Projekte\calculate-emmision-factors\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{722BC5F4-CD6B-46F2-91C2-21091D0902E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A629C95-55AA-48E1-8AF2-40F3D61FE69F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B3864E39-C3D2-F749-9175-08B59E08C58D}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1137" uniqueCount="746">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1289" uniqueCount="802">
   <si>
     <t>Bexbach</t>
   </si>
@@ -2273,6 +2273,174 @@
   </si>
   <si>
     <t>Name BNA</t>
+  </si>
+  <si>
+    <t>Plant Name Smard</t>
+  </si>
+  <si>
+    <t>V_lklingen</t>
+  </si>
+  <si>
+    <t>Trianel_Kohlekraftwerk_L_nen</t>
+  </si>
+  <si>
+    <t>Trianel_Gaskraftwerk_</t>
+  </si>
+  <si>
+    <t>Schwarze_Pumpe</t>
+  </si>
+  <si>
+    <t>Reuter_West</t>
+  </si>
+  <si>
+    <t>Niederau_em</t>
+  </si>
+  <si>
+    <t>M_nchen_Nord_2</t>
+  </si>
+  <si>
+    <t>KWM_Mehrum</t>
+  </si>
+  <si>
+    <t>KWH_Hannover</t>
+  </si>
+  <si>
+    <t>Kraftwerk_Wilhelmshaven</t>
+  </si>
+  <si>
+    <t>Kraftwerk_Walsum</t>
+  </si>
+  <si>
+    <t>Kraftwerk_Walheim</t>
+  </si>
+  <si>
+    <t>Kraftwerk_Voerde</t>
+  </si>
+  <si>
+    <t>Kraftwerk_Mittelsb_ren</t>
+  </si>
+  <si>
+    <t>Kraftwerk_Mainz</t>
+  </si>
+  <si>
+    <t>Kraftwerk_J_nschwalde</t>
+  </si>
+  <si>
+    <t>Kraftwerk_Ingolstadt</t>
+  </si>
+  <si>
+    <t>Kraftwerk_Herne</t>
+  </si>
+  <si>
+    <t>Kraftwerk_Hastedt</t>
+  </si>
+  <si>
+    <t>Kraftwerk_Farge</t>
+  </si>
+  <si>
+    <t>Kraftwerk_Ensdorf</t>
+  </si>
+  <si>
+    <t>Kraftwerk_Bremer_Hafen</t>
+  </si>
+  <si>
+    <t>Kraftwerk_Bexbach</t>
+  </si>
+  <si>
+    <t>Kraftwerk_BASF_Ludwigshafen_S_d</t>
+  </si>
+  <si>
+    <t>Kraftwerk_BASF_Ludwigshafen_Mitte</t>
+  </si>
+  <si>
+    <t>KNG_Kraftwerk_Rostock</t>
+  </si>
+  <si>
+    <t>Knapsack_Gas_II</t>
+  </si>
+  <si>
+    <t>Knapsack_Gas_I</t>
+  </si>
+  <si>
+    <t>K_stenkraftwerk_K.I.E.L.</t>
+  </si>
+  <si>
+    <t>IKS_PCK_Schwedt</t>
+  </si>
+  <si>
+    <t>Ibbenb_ren</t>
+  </si>
+  <si>
+    <t>Huntorf</t>
+  </si>
+  <si>
+    <t>Heizkraftwerk_West_Wolfsburg</t>
+  </si>
+  <si>
+    <t>Heizkraftwerk_R_merbr_cke</t>
+  </si>
+  <si>
+    <t>Heizkraftwerk_Niehl</t>
+  </si>
+  <si>
+    <t>Heizkraftwerk_Merkenich</t>
+  </si>
+  <si>
+    <t>Heizkraftwerk_M_nchen_S_d_GUD2</t>
+  </si>
+  <si>
+    <t>Heizkraftwerk_M_nchen_S_d_GUD1_</t>
+  </si>
+  <si>
+    <t>Heizkraftwerk_Leipzig-Nord</t>
+  </si>
+  <si>
+    <t>Heizkraftwerk_Lausward</t>
+  </si>
+  <si>
+    <t>Heizkraftwerk_Heilbronn</t>
+  </si>
+  <si>
+    <t>Heizkraftwerk_Dresden-Nossener_Br_cke</t>
+  </si>
+  <si>
+    <t>Heizkraftwerk_Altbach_Deizisau</t>
+  </si>
+  <si>
+    <t>GKH_St_cken</t>
+  </si>
+  <si>
+    <t>Gemeinschaftskraftwerk_Kiel</t>
+  </si>
+  <si>
+    <t>Gaskraftwerk_Irsching</t>
+  </si>
+  <si>
+    <t>Franken_1</t>
+  </si>
+  <si>
+    <t>E-Werk_Wilhelmshaven</t>
+  </si>
+  <si>
+    <t>Duisburg_Ruhrort</t>
+  </si>
+  <si>
+    <t>Duisburg_Heizkraftwerk_III</t>
+  </si>
+  <si>
+    <t>Duisburg_Hamborn</t>
+  </si>
+  <si>
+    <t>Cuno_Heizkraftwerk_Herdecke</t>
+  </si>
+  <si>
+    <t>Burghausen_GT</t>
+  </si>
+  <si>
+    <t>Braunkohlekraftwerk_Lippendorf</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -2348,7 +2516,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2358,11 +2526,32 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="15">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -2648,22 +2837,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{849F333F-5B1A-4F37-83E1-1E8DD224AF6E}" name="Tabelle1" displayName="Tabelle1" ref="A1:M152" totalsRowShown="0" headerRowDxfId="13">
-  <autoFilter ref="A1:M152" xr:uid="{849F333F-5B1A-4F37-83E1-1E8DD224AF6E}"/>
-  <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{4F422979-A991-4E34-A517-EFD215C88D16}" name="ETS-ID" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{5F0E830E-86FF-4A7B-99B2-48E60507FF39}" name="EIC" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{0CF3C9A2-B8BF-4625-A90A-A2A85678FFF1}" name="BNA-ID" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{802F1EEC-802C-400C-B743-4D12499B9F49}" name="MaStR-Nr" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{6F4402A2-BFDB-47AC-A995-59F52E01E1AB}" name="Name BNA" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{50C60119-F5E5-45EF-BD10-1589670828EB}" name="City" dataDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{82C3D041-2B42-4975-A236-8BD3A731F36B}" name="Plant name" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{31D64339-73C5-4BE1-A253-730B40AB0E01}" name="Block name" dataDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{E166E0EC-5AEA-49F4-9661-32D6300592B0}" name="CHP" dataDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{7F60C509-592B-4C28-B084-C61CF4E6E4DC}" name="Net electrical power [MW_el]" dataDxfId="3"/>
-    <tableColumn id="11" xr3:uid="{79ADD58E-5FD1-405A-974D-6F314DFCEEEB}" name="Heat power [MW_th]" dataDxfId="2"/>
-    <tableColumn id="12" xr3:uid="{95E443D7-8044-4C17-9A87-C1BB1443F802}" name="Fuel" dataDxfId="1"/>
-    <tableColumn id="13" xr3:uid="{C109E32A-38ED-4594-AF56-CB82B6D69B7F}" name="Fuel emission factor [t/MWh_th]" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{849F333F-5B1A-4F37-83E1-1E8DD224AF6E}" name="Tabelle1" displayName="Tabelle1" ref="A1:N1048576" totalsRowShown="0" headerRowDxfId="14">
+  <autoFilter ref="A1:N1048576" xr:uid="{849F333F-5B1A-4F37-83E1-1E8DD224AF6E}"/>
+  <tableColumns count="14">
+    <tableColumn id="1" xr3:uid="{4F422979-A991-4E34-A517-EFD215C88D16}" name="ETS-ID" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{5F0E830E-86FF-4A7B-99B2-48E60507FF39}" name="EIC" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{0CF3C9A2-B8BF-4625-A90A-A2A85678FFF1}" name="BNA-ID" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{802F1EEC-802C-400C-B743-4D12499B9F49}" name="MaStR-Nr" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{6F4402A2-BFDB-47AC-A995-59F52E01E1AB}" name="Name BNA" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{50C60119-F5E5-45EF-BD10-1589670828EB}" name="City" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{82C3D041-2B42-4975-A236-8BD3A731F36B}" name="Plant name" dataDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{31D64339-73C5-4BE1-A253-730B40AB0E01}" name="Block name" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{E166E0EC-5AEA-49F4-9661-32D6300592B0}" name="CHP" dataDxfId="5"/>
+    <tableColumn id="10" xr3:uid="{7F60C509-592B-4C28-B084-C61CF4E6E4DC}" name="Net electrical power [MW_el]" dataDxfId="4"/>
+    <tableColumn id="11" xr3:uid="{79ADD58E-5FD1-405A-974D-6F314DFCEEEB}" name="Heat power [MW_th]" dataDxfId="3"/>
+    <tableColumn id="12" xr3:uid="{95E443D7-8044-4C17-9A87-C1BB1443F802}" name="Fuel" dataDxfId="2"/>
+    <tableColumn id="13" xr3:uid="{C109E32A-38ED-4594-AF56-CB82B6D69B7F}" name="Fuel emission factor [t/MWh_th]" dataDxfId="1"/>
+    <tableColumn id="15" xr3:uid="{C77CDCD9-C0EF-4845-A7F6-BB13EE0F371C}" name="Plant Name Smard" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2966,31 +3156,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ACF6D7F-52CF-D341-876A-D8AC559D8C06}">
-  <dimension ref="A1:M152"/>
+  <dimension ref="A1:N152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="74" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S66" sqref="S66"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="74" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N2" sqref="N1:N1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8" customWidth="1"/>
-    <col min="2" max="2" width="21.296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.69921875" customWidth="1"/>
-    <col min="4" max="4" width="19.19921875" customWidth="1"/>
-    <col min="5" max="5" width="48.19921875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.09765625" customWidth="1"/>
-    <col min="7" max="7" width="16.5" customWidth="1"/>
-    <col min="8" max="8" width="15.8984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.69921875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="31.69921875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.296875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.296875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="34.296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8" style="1" customWidth="1"/>
+    <col min="2" max="2" width="21.296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.69921875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.19921875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="48.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.09765625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.8984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.69921875" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="31.69921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="34.296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="39.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
@@ -3030,8 +3221,11 @@
       <c r="M1" s="3" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N1" s="5" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1399</v>
       </c>
@@ -3071,8 +3265,11 @@
       <c r="M2" s="1">
         <v>0.33679999999999999</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N2" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1453</v>
       </c>
@@ -3112,8 +3309,11 @@
       <c r="M3" s="1">
         <v>0.39800000000000002</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N3" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>1453</v>
       </c>
@@ -3153,8 +3353,11 @@
       <c r="M4" s="1">
         <v>0.39800000000000002</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N4" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>1454</v>
       </c>
@@ -3194,8 +3397,11 @@
       <c r="M5" s="1">
         <v>0.39800000000000002</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N5" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1454</v>
       </c>
@@ -3235,8 +3441,11 @@
       <c r="M6" s="1">
         <v>0.39800000000000002</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N6" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>1460</v>
       </c>
@@ -3276,8 +3485,11 @@
       <c r="M7" s="1">
         <v>0.37169999999999997</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N7" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>1460</v>
       </c>
@@ -3317,8 +3529,11 @@
       <c r="M8" s="1">
         <v>0.37169999999999997</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N8" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>795</v>
       </c>
@@ -3340,7 +3555,6 @@
       <c r="G9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H9" s="2"/>
       <c r="I9" s="2">
         <v>1</v>
       </c>
@@ -3356,8 +3570,11 @@
       <c r="M9" s="1">
         <v>0.20100000000000001</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N9" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>1419</v>
       </c>
@@ -3367,7 +3584,6 @@
       <c r="C10" s="1" t="s">
         <v>455</v>
       </c>
-      <c r="D10" s="1"/>
       <c r="E10" s="1" t="s">
         <v>166</v>
       </c>
@@ -3377,7 +3593,6 @@
       <c r="G10" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="H10" s="2"/>
       <c r="I10" s="2">
         <v>0</v>
       </c>
@@ -3393,8 +3608,11 @@
       <c r="M10" s="1">
         <v>0.35820000000000002</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N10" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>1409</v>
       </c>
@@ -3434,8 +3652,11 @@
       <c r="M11" s="1">
         <v>0.20100000000000001</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N11" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>208968</v>
       </c>
@@ -3475,8 +3696,11 @@
       <c r="M12" s="1">
         <v>0.33679999999999999</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N12" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>1485</v>
       </c>
@@ -3516,8 +3740,11 @@
       <c r="M13" s="1">
         <v>0.20100000000000001</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N13" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>1411</v>
       </c>
@@ -3548,15 +3775,17 @@
       <c r="J14" s="1">
         <v>100</v>
       </c>
-      <c r="K14" s="1"/>
       <c r="L14" s="1" t="s">
         <v>8</v>
       </c>
       <c r="M14" s="1">
         <v>0.93189999999999995</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N14" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>1850</v>
       </c>
@@ -3596,8 +3825,11 @@
       <c r="M15" s="1">
         <v>0.93189999999999995</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N15" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>1174</v>
       </c>
@@ -3637,8 +3869,11 @@
       <c r="M16" s="1">
         <v>0.20100000000000001</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N16" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>1415</v>
       </c>
@@ -3669,15 +3904,17 @@
       <c r="J17" s="1">
         <v>165</v>
       </c>
-      <c r="K17" s="1"/>
       <c r="L17" s="1" t="s">
         <v>8</v>
       </c>
       <c r="M17" s="1">
         <v>0.93189999999999995</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N17" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>1479</v>
       </c>
@@ -3717,8 +3954,11 @@
       <c r="M18" s="1">
         <v>0.20100000000000001</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N18" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>1479</v>
       </c>
@@ -3758,8 +3998,11 @@
       <c r="M19" s="1">
         <v>0.20100000000000001</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N19" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>1479</v>
       </c>
@@ -3799,8 +4042,11 @@
       <c r="M20" s="1">
         <v>0.20100000000000001</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N20" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>969</v>
       </c>
@@ -3810,7 +4056,6 @@
       <c r="C21" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="D21" s="1"/>
       <c r="E21" s="1" t="s">
         <v>725</v>
       </c>
@@ -3820,7 +4065,6 @@
       <c r="G21" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="H21" s="2"/>
       <c r="I21" s="2">
         <v>0</v>
       </c>
@@ -3836,8 +4080,11 @@
       <c r="M21" s="1">
         <v>0.33679999999999999</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N21" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>1446</v>
       </c>
@@ -3877,8 +4124,11 @@
       <c r="M22" s="1">
         <v>0.20100000000000001</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N22" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>1446</v>
       </c>
@@ -3918,8 +4168,11 @@
       <c r="M23" s="1">
         <v>0.20100000000000001</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N23" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>1605</v>
       </c>
@@ -3929,7 +4182,6 @@
       <c r="C24" s="1" t="s">
         <v>464</v>
       </c>
-      <c r="D24" s="1"/>
       <c r="E24" s="1" t="s">
         <v>733</v>
       </c>
@@ -3957,8 +4209,11 @@
       <c r="M24" s="1">
         <v>0.40749999999999997</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N24" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>1605</v>
       </c>
@@ -3968,7 +4223,6 @@
       <c r="C25" s="1" t="s">
         <v>465</v>
       </c>
-      <c r="D25" s="1"/>
       <c r="E25" s="1" t="s">
         <v>734</v>
       </c>
@@ -3996,8 +4250,11 @@
       <c r="M25" s="1">
         <v>0.40749999999999997</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N25" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>1207</v>
       </c>
@@ -4037,8 +4294,11 @@
       <c r="M26" s="1">
         <v>0.26640000000000003</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N26" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>4148</v>
       </c>
@@ -4078,8 +4338,11 @@
       <c r="M27" s="1">
         <v>0.20100000000000001</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N27" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>1207</v>
       </c>
@@ -4119,8 +4382,11 @@
       <c r="M28" s="1">
         <v>0.20100000000000001</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N28" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>1210</v>
       </c>
@@ -4130,7 +4396,6 @@
       <c r="C29" s="1" t="s">
         <v>453</v>
       </c>
-      <c r="D29" s="1"/>
       <c r="E29" s="1" t="s">
         <v>727</v>
       </c>
@@ -4140,7 +4405,6 @@
       <c r="G29" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="H29" s="2"/>
       <c r="I29" s="2">
         <v>1</v>
       </c>
@@ -4156,8 +4420,11 @@
       <c r="M29" s="1">
         <v>0.33679999999999999</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N29" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>1481</v>
       </c>
@@ -4197,8 +4464,11 @@
       <c r="M30" s="1">
         <v>0.33679999999999999</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N30" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>1481</v>
       </c>
@@ -4238,8 +4508,11 @@
       <c r="M31" s="1">
         <v>0.20100000000000001</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N31" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>1481</v>
       </c>
@@ -4279,8 +4552,11 @@
       <c r="M32" s="1">
         <v>0.20100000000000001</v>
       </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N32" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>1481</v>
       </c>
@@ -4320,8 +4596,11 @@
       <c r="M33" s="1">
         <v>0.20100000000000001</v>
       </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N33" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>1481</v>
       </c>
@@ -4361,8 +4640,11 @@
       <c r="M34" s="1">
         <v>0.20100000000000001</v>
       </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N34" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>1387</v>
       </c>
@@ -4402,8 +4684,11 @@
       <c r="M35" s="1">
         <v>0.33679999999999999</v>
       </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N35" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>1387</v>
       </c>
@@ -4443,8 +4728,11 @@
       <c r="M36" s="1">
         <v>0.33679999999999999</v>
       </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N36" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>1450</v>
       </c>
@@ -4484,8 +4772,11 @@
       <c r="M37" s="1">
         <v>0.33679999999999999</v>
       </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N37" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>1450</v>
       </c>
@@ -4525,8 +4816,11 @@
       <c r="M38" s="1">
         <v>0.33679999999999999</v>
       </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N38" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>739</v>
       </c>
@@ -4548,7 +4842,6 @@
       <c r="G39" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="H39" s="2"/>
       <c r="I39" s="2">
         <v>1</v>
       </c>
@@ -4564,8 +4857,11 @@
       <c r="M39" s="1">
         <v>0.20100000000000001</v>
       </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N39" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>1452</v>
       </c>
@@ -4605,8 +4901,11 @@
       <c r="M40" s="1">
         <v>0.33679999999999999</v>
       </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N40" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>1095</v>
       </c>
@@ -4646,8 +4945,11 @@
       <c r="M41" s="1">
         <v>0.20100000000000001</v>
       </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N41" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>1095</v>
       </c>
@@ -4687,8 +4989,11 @@
       <c r="M42" s="1">
         <v>0.20100000000000001</v>
       </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N42" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>1095</v>
       </c>
@@ -4728,8 +5033,11 @@
       <c r="M43" s="1">
         <v>0.20100000000000001</v>
       </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N43" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>1444</v>
       </c>
@@ -4751,7 +5059,6 @@
       <c r="G44" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="H44" s="2"/>
       <c r="I44" s="2">
         <v>1</v>
       </c>
@@ -4767,8 +5074,11 @@
       <c r="M44" s="1">
         <v>0.20100000000000001</v>
       </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N44" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>750</v>
       </c>
@@ -4808,8 +5118,11 @@
       <c r="M45" s="1">
         <v>0.20100000000000001</v>
       </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N45" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>750</v>
       </c>
@@ -4849,8 +5162,11 @@
       <c r="M46" s="1">
         <v>0.20100000000000001</v>
       </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N46" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>750</v>
       </c>
@@ -4890,8 +5206,11 @@
       <c r="M47" s="1">
         <v>0.20100000000000001</v>
       </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N47" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>750</v>
       </c>
@@ -4931,8 +5250,11 @@
       <c r="M48" s="1">
         <v>0.20100000000000001</v>
       </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N48" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>750</v>
       </c>
@@ -4972,8 +5294,11 @@
       <c r="M49" s="1">
         <v>0.20100000000000001</v>
       </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N49" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>1276</v>
       </c>
@@ -5013,8 +5338,11 @@
       <c r="M50" s="1">
         <v>0.20100000000000001</v>
       </c>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N50" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>1279</v>
       </c>
@@ -5054,8 +5382,11 @@
       <c r="M51" s="1">
         <v>0.20100000000000001</v>
       </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N51" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>1279</v>
       </c>
@@ -5095,8 +5426,11 @@
       <c r="M52" s="1">
         <v>0.20100000000000001</v>
       </c>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N52" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>1279</v>
       </c>
@@ -5136,8 +5470,11 @@
       <c r="M53" s="1">
         <v>0.20100000000000001</v>
       </c>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N53" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>1746</v>
       </c>
@@ -5177,8 +5514,11 @@
       <c r="M54" s="1">
         <v>0.20100000000000001</v>
       </c>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N54" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>1515</v>
       </c>
@@ -5218,8 +5558,11 @@
       <c r="M55" s="1">
         <v>0.33679999999999999</v>
       </c>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N55" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>1515</v>
       </c>
@@ -5259,8 +5602,11 @@
       <c r="M56" s="1">
         <v>0.33679999999999999</v>
       </c>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N56" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>1291</v>
       </c>
@@ -5282,7 +5628,6 @@
       <c r="G57" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="H57" s="2"/>
       <c r="I57" s="2">
         <v>0</v>
       </c>
@@ -5298,8 +5643,11 @@
       <c r="M57" s="1">
         <v>0.33679999999999999</v>
       </c>
-    </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N57" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>1486</v>
       </c>
@@ -5339,8 +5687,11 @@
       <c r="M58" s="1">
         <v>0.93189999999999995</v>
       </c>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N58" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>1486</v>
       </c>
@@ -5380,8 +5731,11 @@
       <c r="M59" s="1">
         <v>0.93189999999999995</v>
       </c>
-    </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N59" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>995</v>
       </c>
@@ -5403,7 +5757,6 @@
       <c r="G60" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="H60" s="2"/>
       <c r="I60" s="2">
         <v>0</v>
       </c>
@@ -5419,8 +5772,11 @@
       <c r="M60" s="1">
         <v>0.20100000000000001</v>
       </c>
-    </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N60" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>1480</v>
       </c>
@@ -5430,7 +5786,6 @@
       <c r="C61" s="1" t="s">
         <v>410</v>
       </c>
-      <c r="D61" s="1"/>
       <c r="E61" s="1" t="s">
         <v>731</v>
       </c>
@@ -5458,8 +5813,11 @@
       <c r="M61" s="1">
         <v>0.33679999999999999</v>
       </c>
-    </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N61" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>19</v>
       </c>
@@ -5499,8 +5857,11 @@
       <c r="M62" s="1">
         <v>0.26390000000000002</v>
       </c>
-    </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N62" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>19</v>
       </c>
@@ -5540,8 +5901,11 @@
       <c r="M63" s="1">
         <v>0.26390000000000002</v>
       </c>
-    </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N63" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>210483</v>
       </c>
@@ -5563,7 +5927,6 @@
       <c r="G64" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="H64" s="2"/>
       <c r="I64" s="1">
         <v>1</v>
       </c>
@@ -5579,8 +5942,11 @@
       <c r="M64" s="1">
         <v>0.20100000000000001</v>
       </c>
-    </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N64" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <v>1170</v>
       </c>
@@ -5602,7 +5968,6 @@
       <c r="G65" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="H65" s="2"/>
       <c r="I65" s="2">
         <v>1</v>
       </c>
@@ -5618,8 +5983,11 @@
       <c r="M65" s="1">
         <v>0.20100000000000001</v>
       </c>
-    </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N65" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>1786</v>
       </c>
@@ -5659,8 +6027,11 @@
       <c r="M66" s="1">
         <v>0.20100000000000001</v>
       </c>
-    </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N66" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <v>202777</v>
       </c>
@@ -5700,8 +6071,11 @@
       <c r="M67" s="1">
         <v>0.20100000000000001</v>
       </c>
-    </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N67" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>1309</v>
       </c>
@@ -5723,7 +6097,6 @@
       <c r="G68" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H68" s="2"/>
       <c r="I68" s="2">
         <v>1</v>
       </c>
@@ -5739,8 +6112,11 @@
       <c r="M68" s="1">
         <v>0.33679999999999999</v>
       </c>
-    </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N68" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <v>662</v>
       </c>
@@ -5780,8 +6156,11 @@
       <c r="M69" s="1">
         <v>0.20100000000000001</v>
       </c>
-    </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N69" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <v>662</v>
       </c>
@@ -5821,8 +6200,11 @@
       <c r="M70" s="1">
         <v>0.20100000000000001</v>
       </c>
-    </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N70" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <v>1484</v>
       </c>
@@ -5862,8 +6244,11 @@
       <c r="M71" s="1">
         <v>0.20100000000000001</v>
       </c>
-    </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N71" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <v>1484</v>
       </c>
@@ -5903,8 +6288,11 @@
       <c r="M72" s="1">
         <v>0.20100000000000001</v>
       </c>
-    </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N72" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <v>852</v>
       </c>
@@ -5944,8 +6332,11 @@
       <c r="M73" s="1">
         <v>0.33679999999999999</v>
       </c>
-    </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N73" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <v>1238</v>
       </c>
@@ -5955,7 +6346,6 @@
       <c r="C74" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="D74" s="1"/>
       <c r="E74" s="1" t="s">
         <v>728</v>
       </c>
@@ -5983,8 +6373,11 @@
       <c r="M74" s="1">
         <v>0.33679999999999999</v>
       </c>
-    </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N74" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <v>839</v>
       </c>
@@ -5994,7 +6387,6 @@
       <c r="C75" s="1" t="s">
         <v>449</v>
       </c>
-      <c r="D75" s="1"/>
       <c r="E75" s="1" t="s">
         <v>724</v>
       </c>
@@ -6013,15 +6405,17 @@
       <c r="J75" s="1">
         <v>106</v>
       </c>
-      <c r="K75" s="1"/>
       <c r="L75" s="1" t="s">
         <v>7</v>
       </c>
       <c r="M75" s="1">
         <v>0.33679999999999999</v>
       </c>
-    </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N75" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <v>838</v>
       </c>
@@ -6031,7 +6425,6 @@
       <c r="C76" s="1" t="s">
         <v>450</v>
       </c>
-      <c r="D76" s="1"/>
       <c r="E76" s="1" t="s">
         <v>724</v>
       </c>
@@ -6059,8 +6452,11 @@
       <c r="M76" s="1">
         <v>0.33679999999999999</v>
       </c>
-    </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N76" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <v>999</v>
       </c>
@@ -6082,7 +6478,6 @@
       <c r="G77" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="H77" s="2"/>
       <c r="I77" s="2">
         <v>0</v>
       </c>
@@ -6098,8 +6493,11 @@
       <c r="M77" s="1">
         <v>0.33679999999999999</v>
       </c>
-    </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N77" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <v>1253</v>
       </c>
@@ -6139,8 +6537,11 @@
       <c r="M78" s="1">
         <v>0.33679999999999999</v>
       </c>
-    </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N78" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
         <v>1312</v>
       </c>
@@ -6180,8 +6581,11 @@
       <c r="M79" s="1">
         <v>0.33679999999999999</v>
       </c>
-    </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N79" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
         <v>1447</v>
       </c>
@@ -6221,8 +6625,11 @@
       <c r="M80" s="1">
         <v>0.28910000000000002</v>
       </c>
-    </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N80" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="81" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
         <v>1447</v>
       </c>
@@ -6262,8 +6669,11 @@
       <c r="M81" s="1">
         <v>0.28910000000000002</v>
       </c>
-    </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N81" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="82" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
         <v>1456</v>
       </c>
@@ -6303,8 +6713,11 @@
       <c r="M82" s="1">
         <v>0.39800000000000002</v>
       </c>
-    </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N82" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
         <v>1456</v>
       </c>
@@ -6344,8 +6757,11 @@
       <c r="M83" s="1">
         <v>0.39800000000000002</v>
       </c>
-    </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N83" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="84" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
         <v>1456</v>
       </c>
@@ -6385,8 +6801,11 @@
       <c r="M84" s="1">
         <v>0.39800000000000002</v>
       </c>
-    </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N84" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="85" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
         <v>1456</v>
       </c>
@@ -6426,8 +6845,11 @@
       <c r="M85" s="1">
         <v>0.39800000000000002</v>
       </c>
-    </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N85" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="86" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
         <v>1456</v>
       </c>
@@ -6458,15 +6880,17 @@
       <c r="J86" s="1">
         <v>500</v>
       </c>
-      <c r="K86" s="1"/>
       <c r="L86" s="1" t="s">
         <v>6</v>
       </c>
       <c r="M86" s="1">
         <v>0.39800000000000002</v>
       </c>
-    </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N86" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="87" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
         <v>1456</v>
       </c>
@@ -6497,15 +6921,17 @@
       <c r="J87" s="1">
         <v>498</v>
       </c>
-      <c r="K87" s="1"/>
       <c r="L87" s="1" t="s">
         <v>6</v>
       </c>
       <c r="M87" s="1">
         <v>0.39800000000000002</v>
       </c>
-    </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N87" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="88" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
         <v>1064</v>
       </c>
@@ -6545,8 +6971,11 @@
       <c r="M88" s="1">
         <v>0.20100000000000001</v>
       </c>
-    </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N88" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="89" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
         <v>1064</v>
       </c>
@@ -6586,8 +7015,11 @@
       <c r="M89" s="1">
         <v>0.20100000000000001</v>
       </c>
-    </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N89" t="s">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="90" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
         <v>1228</v>
       </c>
@@ -6627,8 +7059,11 @@
       <c r="M90" s="1">
         <v>0.93189999999999995</v>
       </c>
-    </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N90" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
         <v>1318</v>
       </c>
@@ -6638,7 +7073,6 @@
       <c r="C91" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="D91" s="1"/>
       <c r="E91" s="1" t="s">
         <v>732</v>
       </c>
@@ -6666,8 +7100,11 @@
       <c r="M91" s="1">
         <v>0.33679999999999999</v>
       </c>
-    </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N91" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="92" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
         <v>1318</v>
       </c>
@@ -6677,7 +7114,6 @@
       <c r="C92" s="1" t="s">
         <v>463</v>
       </c>
-      <c r="D92" s="1"/>
       <c r="E92" s="1" t="s">
         <v>732</v>
       </c>
@@ -6705,8 +7141,11 @@
       <c r="M92" s="1">
         <v>0.33679999999999999</v>
       </c>
-    </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N92" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="93" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A93" s="1">
         <v>1464</v>
       </c>
@@ -6746,8 +7185,11 @@
       <c r="M93" s="1">
         <v>0.26640000000000003</v>
       </c>
-    </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N93" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="94" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
         <v>1317</v>
       </c>
@@ -6787,8 +7229,11 @@
       <c r="M94" s="1">
         <v>0.33679999999999999</v>
       </c>
-    </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N94" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="95" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A95" s="1">
         <v>1317</v>
       </c>
@@ -6798,7 +7243,6 @@
       <c r="C95" s="1" t="s">
         <v>377</v>
       </c>
-      <c r="D95" s="1"/>
       <c r="E95" s="1" t="s">
         <v>729</v>
       </c>
@@ -6826,8 +7270,11 @@
       <c r="M95" s="1">
         <v>0.33679999999999999</v>
       </c>
-    </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N95" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="96" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A96" s="1">
         <v>205778</v>
       </c>
@@ -6849,7 +7296,6 @@
       <c r="G96" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="H96" s="2"/>
       <c r="I96" s="2">
         <v>0</v>
       </c>
@@ -6865,8 +7311,11 @@
       <c r="M96" s="1">
         <v>0.33679999999999999</v>
       </c>
-    </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N96" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="97" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A97" s="1">
         <v>1384</v>
       </c>
@@ -6876,7 +7325,6 @@
       <c r="C97" s="1" t="s">
         <v>380</v>
       </c>
-      <c r="D97" s="1"/>
       <c r="E97" s="1" t="s">
         <v>730</v>
       </c>
@@ -6904,8 +7352,11 @@
       <c r="M97" s="1">
         <v>0.20100000000000001</v>
       </c>
-    </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N97" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="98" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A98" s="1">
         <v>939</v>
       </c>
@@ -6945,8 +7396,11 @@
       <c r="M98" s="1">
         <v>0.33679999999999999</v>
       </c>
-    </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N98" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="99" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A99" s="1">
         <v>209842</v>
       </c>
@@ -6986,8 +7440,11 @@
       <c r="M99" s="1">
         <v>0.20100000000000001</v>
       </c>
-    </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N99" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="100" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A100" s="1">
         <v>209842</v>
       </c>
@@ -6997,7 +7454,6 @@
       <c r="C100" s="1" t="s">
         <v>470</v>
       </c>
-      <c r="D100" s="1"/>
       <c r="E100" s="1" t="s">
         <v>297</v>
       </c>
@@ -7025,8 +7481,11 @@
       <c r="M100" s="1">
         <v>0.20100000000000001</v>
       </c>
-    </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N100" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="101" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A101" s="1">
         <v>209842</v>
       </c>
@@ -7036,7 +7495,6 @@
       <c r="C101" s="1" t="s">
         <v>471</v>
       </c>
-      <c r="D101" s="1"/>
       <c r="E101" s="1" t="s">
         <v>297</v>
       </c>
@@ -7064,8 +7522,11 @@
       <c r="M101" s="1">
         <v>0.20100000000000001</v>
       </c>
-    </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N101" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="102" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A102" s="1">
         <v>741</v>
       </c>
@@ -7105,8 +7566,11 @@
       <c r="M102" s="1">
         <v>0.33679999999999999</v>
       </c>
-    </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N102" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="103" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A103" s="1">
         <v>206180</v>
       </c>
@@ -7116,7 +7580,6 @@
       <c r="C103" s="1" t="s">
         <v>444</v>
       </c>
-      <c r="D103" s="1"/>
       <c r="E103" s="1" t="s">
         <v>740</v>
       </c>
@@ -7144,8 +7607,11 @@
       <c r="M103" s="1">
         <v>0.33679999999999999</v>
       </c>
-    </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N103" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="104" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A104" s="1">
         <v>206180</v>
       </c>
@@ -7155,7 +7621,6 @@
       <c r="C104" s="1" t="s">
         <v>445</v>
       </c>
-      <c r="D104" s="1"/>
       <c r="E104" s="1" t="s">
         <v>741</v>
       </c>
@@ -7183,8 +7648,11 @@
       <c r="M104" s="1">
         <v>0.33679999999999999</v>
       </c>
-    </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N104" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="105" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A105" s="1">
         <v>1606</v>
       </c>
@@ -7224,8 +7692,11 @@
       <c r="M105" s="1">
         <v>0.40749999999999997</v>
       </c>
-    </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N105" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="106" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A106" s="1">
         <v>1606</v>
       </c>
@@ -7265,8 +7736,11 @@
       <c r="M106" s="1">
         <v>0.40749999999999997</v>
       </c>
-    </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N106" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="107" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A107" s="1">
         <v>1606</v>
       </c>
@@ -7276,7 +7750,6 @@
       <c r="C107" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="D107" s="1"/>
       <c r="E107" s="1" t="s">
         <v>735</v>
       </c>
@@ -7304,8 +7777,11 @@
       <c r="M107" s="1">
         <v>0.40749999999999997</v>
       </c>
-    </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N107" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="108" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A108" s="1">
         <v>1606</v>
       </c>
@@ -7345,8 +7821,11 @@
       <c r="M108" s="1">
         <v>0.40749999999999997</v>
       </c>
-    </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N108" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="109" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A109" s="1">
         <v>1606</v>
       </c>
@@ -7386,8 +7865,11 @@
       <c r="M109" s="1">
         <v>0.40749999999999997</v>
       </c>
-    </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N109" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="110" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A110" s="1">
         <v>1606</v>
       </c>
@@ -7427,8 +7909,11 @@
       <c r="M110" s="1">
         <v>0.40749999999999997</v>
       </c>
-    </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N110" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="111" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A111" s="1">
         <v>1606</v>
       </c>
@@ -7468,8 +7953,11 @@
       <c r="M111" s="1">
         <v>0.40749999999999997</v>
       </c>
-    </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N111" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="112" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A112" s="1">
         <v>1649</v>
       </c>
@@ -7509,8 +7997,11 @@
       <c r="M112" s="1">
         <v>0.40749999999999997</v>
       </c>
-    </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N112" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="113" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A113" s="1">
         <v>1649</v>
       </c>
@@ -7541,15 +8032,17 @@
       <c r="J113" s="1">
         <v>639</v>
       </c>
-      <c r="K113" s="1"/>
       <c r="L113" s="1" t="s">
         <v>6</v>
       </c>
       <c r="M113" s="1">
         <v>0.40749999999999997</v>
       </c>
-    </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N113" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="114" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A114" s="1">
         <v>1649</v>
       </c>
@@ -7580,15 +8073,17 @@
       <c r="J114" s="1">
         <v>924</v>
       </c>
-      <c r="K114" s="1"/>
       <c r="L114" s="1" t="s">
         <v>6</v>
       </c>
       <c r="M114" s="1">
         <v>0.40749999999999997</v>
       </c>
-    </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N114" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="115" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A115" s="1">
         <v>1649</v>
       </c>
@@ -7598,7 +8093,6 @@
       <c r="C115" s="1" t="s">
         <v>432</v>
       </c>
-      <c r="D115" s="1"/>
       <c r="E115" s="1" t="s">
         <v>737</v>
       </c>
@@ -7617,15 +8111,17 @@
       <c r="J115" s="1">
         <v>296</v>
       </c>
-      <c r="K115" s="1"/>
       <c r="L115" s="1" t="s">
         <v>6</v>
       </c>
       <c r="M115" s="1">
         <v>0.40749999999999997</v>
       </c>
-    </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N115" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="116" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A116" s="1">
         <v>1649</v>
       </c>
@@ -7635,7 +8131,6 @@
       <c r="C116" s="1" t="s">
         <v>594</v>
       </c>
-      <c r="D116" s="1"/>
       <c r="E116" s="1" t="s">
         <v>738</v>
       </c>
@@ -7654,15 +8149,17 @@
       <c r="J116" s="1">
         <v>301</v>
       </c>
-      <c r="K116" s="1"/>
       <c r="L116" s="1" t="s">
         <v>6</v>
       </c>
       <c r="M116" s="1">
         <v>0.40749999999999997</v>
       </c>
-    </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N116" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="117" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A117" s="1">
         <v>1649</v>
       </c>
@@ -7693,15 +8190,17 @@
       <c r="J117" s="1">
         <v>307</v>
       </c>
-      <c r="K117" s="1"/>
       <c r="L117" s="1" t="s">
         <v>6</v>
       </c>
       <c r="M117" s="1">
         <v>0.40749999999999997</v>
       </c>
-    </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N117" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="118" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A118" s="1">
         <v>1649</v>
       </c>
@@ -7741,8 +8240,11 @@
       <c r="M118" s="1">
         <v>0.40749999999999997</v>
       </c>
-    </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N118" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="119" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A119" s="1">
         <v>1181</v>
       </c>
@@ -7752,7 +8254,6 @@
       <c r="C119" s="1" t="s">
         <v>454</v>
       </c>
-      <c r="D119" s="1"/>
       <c r="E119" s="1" t="s">
         <v>726</v>
       </c>
@@ -7780,8 +8281,11 @@
       <c r="M119" s="1">
         <v>0.33679999999999999</v>
       </c>
-    </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N119" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="120" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A120" s="1">
         <v>1179</v>
       </c>
@@ -7821,8 +8325,11 @@
       <c r="M120" s="1">
         <v>0.33679999999999999</v>
       </c>
-    </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N120" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="121" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A121" s="1">
         <v>1179</v>
       </c>
@@ -7862,8 +8369,11 @@
       <c r="M121" s="1">
         <v>0.33679999999999999</v>
       </c>
-    </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N121" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="122" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A122" s="1">
         <v>1457</v>
       </c>
@@ -7903,8 +8413,11 @@
       <c r="M122" s="1">
         <v>0.33679999999999999</v>
       </c>
-    </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N122" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="123" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A123" s="1">
         <v>1457</v>
       </c>
@@ -7944,8 +8457,11 @@
       <c r="M123" s="1">
         <v>0.33679999999999999</v>
       </c>
-    </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N123" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="124" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A124" s="1">
         <v>1457</v>
       </c>
@@ -7985,8 +8501,11 @@
       <c r="M124" s="1">
         <v>0.20100000000000001</v>
       </c>
-    </row>
-    <row r="125" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N124" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="125" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A125" s="1">
         <v>1376</v>
       </c>
@@ -8026,8 +8545,11 @@
       <c r="M125" s="1">
         <v>0.37169999999999997</v>
       </c>
-    </row>
-    <row r="126" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N125" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="126" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A126" s="1">
         <v>1376</v>
       </c>
@@ -8067,8 +8589,11 @@
       <c r="M126" s="1">
         <v>0.37169999999999997</v>
       </c>
-    </row>
-    <row r="127" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N126" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="127" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A127" s="1">
         <v>1205</v>
       </c>
@@ -8099,15 +8624,17 @@
       <c r="J127" s="1">
         <v>345</v>
       </c>
-      <c r="K127" s="1"/>
       <c r="L127" s="1" t="s">
         <v>7</v>
       </c>
       <c r="M127" s="1">
         <v>0.33679999999999999</v>
       </c>
-    </row>
-    <row r="128" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N127" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="128" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A128" s="1">
         <v>1205</v>
       </c>
@@ -8138,15 +8665,17 @@
       <c r="J128" s="1">
         <v>345</v>
       </c>
-      <c r="K128" s="1"/>
       <c r="L128" s="1" t="s">
         <v>7</v>
       </c>
       <c r="M128" s="1">
         <v>0.33679999999999999</v>
       </c>
-    </row>
-    <row r="129" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N128" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="129" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A129" s="1">
         <v>1459</v>
       </c>
@@ -8186,8 +8715,11 @@
       <c r="M129" s="1">
         <v>0.39800000000000002</v>
       </c>
-    </row>
-    <row r="130" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N129" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="130" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A130" s="1">
         <v>1459</v>
       </c>
@@ -8227,8 +8759,11 @@
       <c r="M130" s="1">
         <v>0.39800000000000002</v>
       </c>
-    </row>
-    <row r="131" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N130" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="131" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A131" s="1">
         <v>1876</v>
       </c>
@@ -8268,10 +8803,13 @@
       <c r="M131" s="1">
         <v>0.33679999999999999</v>
       </c>
-    </row>
-    <row r="132" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N131" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="132" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A132" s="1">
-        <v>1379</v>
+        <v>1876</v>
       </c>
       <c r="B132" s="1" t="s">
         <v>67</v>
@@ -8309,8 +8847,11 @@
       <c r="M132" s="1">
         <v>0.33679999999999999</v>
       </c>
-    </row>
-    <row r="133" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N132" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="133" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A133" s="1">
         <v>951</v>
       </c>
@@ -8350,8 +8891,11 @@
       <c r="M133" s="1">
         <v>0.33679999999999999</v>
       </c>
-    </row>
-    <row r="134" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N133" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="134" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A134" s="1">
         <v>951</v>
       </c>
@@ -8391,8 +8935,11 @@
       <c r="M134" s="1">
         <v>0.20100000000000001</v>
       </c>
-    </row>
-    <row r="135" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N134" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="135" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A135" s="1">
         <v>2195</v>
       </c>
@@ -8432,8 +8979,11 @@
       <c r="M135" s="1">
         <v>0.20100000000000001</v>
       </c>
-    </row>
-    <row r="136" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N135" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="136" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A136" s="1">
         <v>2195</v>
       </c>
@@ -8473,8 +9023,11 @@
       <c r="M136" s="1">
         <v>0.20100000000000001</v>
       </c>
-    </row>
-    <row r="137" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N136" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="137" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A137" s="1">
         <v>4166</v>
       </c>
@@ -8514,8 +9067,11 @@
       <c r="M137" s="1">
         <v>0.33679999999999999</v>
       </c>
-    </row>
-    <row r="138" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N137" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="138" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>889</v>
       </c>
@@ -8555,8 +9111,11 @@
       <c r="M138" s="1">
         <v>0.33679999999999999</v>
       </c>
-    </row>
-    <row r="139" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N138" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="139" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A139" s="1">
         <v>851</v>
       </c>
@@ -8596,8 +9155,11 @@
       <c r="M139" s="1">
         <v>0.33679999999999999</v>
       </c>
-    </row>
-    <row r="140" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N139" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="140" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A140" s="1">
         <v>952</v>
       </c>
@@ -8637,8 +9199,11 @@
       <c r="M140" s="1">
         <v>0.33679999999999999</v>
       </c>
-    </row>
-    <row r="141" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N140" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="141" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A141" s="1">
         <v>952</v>
       </c>
@@ -8678,8 +9243,11 @@
       <c r="M141" s="1">
         <v>0.33679999999999999</v>
       </c>
-    </row>
-    <row r="142" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N141" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="142" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A142" s="1">
         <v>845</v>
       </c>
@@ -8719,8 +9287,11 @@
       <c r="M142" s="1">
         <v>0.33679999999999999</v>
       </c>
-    </row>
-    <row r="143" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N142" t="s">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="143" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A143" s="1">
         <v>1607</v>
       </c>
@@ -8760,8 +9331,11 @@
       <c r="M143" s="1">
         <v>0.40749999999999997</v>
       </c>
-    </row>
-    <row r="144" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N143" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="144" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A144" s="1">
         <v>1607</v>
       </c>
@@ -8801,8 +9375,11 @@
       <c r="M144" s="1">
         <v>0.40749999999999997</v>
       </c>
-    </row>
-    <row r="145" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N144" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="145" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A145" s="1">
         <v>1607</v>
       </c>
@@ -8842,8 +9419,11 @@
       <c r="M145" s="1">
         <v>0.40749999999999997</v>
       </c>
-    </row>
-    <row r="146" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N145" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="146" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A146" s="1">
         <v>1607</v>
       </c>
@@ -8853,7 +9433,6 @@
       <c r="C146" s="1" t="s">
         <v>426</v>
       </c>
-      <c r="D146" s="1"/>
       <c r="E146" s="1" t="s">
         <v>736</v>
       </c>
@@ -8881,8 +9460,11 @@
       <c r="M146" s="1">
         <v>0.40749999999999997</v>
       </c>
-    </row>
-    <row r="147" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N146" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="147" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A147" s="1">
         <v>1607</v>
       </c>
@@ -8922,8 +9504,11 @@
       <c r="M147" s="1">
         <v>0.20100000000000001</v>
       </c>
-    </row>
-    <row r="148" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N147" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="148" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A148" s="1">
         <v>1607</v>
       </c>
@@ -8963,8 +9548,11 @@
       <c r="M148" s="1">
         <v>0.20100000000000001</v>
       </c>
-    </row>
-    <row r="149" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N148" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="149" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A149" s="1">
         <v>1474</v>
       </c>
@@ -8974,7 +9562,6 @@
       <c r="C149" s="1" t="s">
         <v>469</v>
       </c>
-      <c r="D149" s="1"/>
       <c r="E149" s="1" t="s">
         <v>285</v>
       </c>
@@ -9002,8 +9589,11 @@
       <c r="M149" s="1">
         <v>0.33679999999999999</v>
       </c>
-    </row>
-    <row r="150" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N149" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="150" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A150" s="1">
         <v>1474</v>
       </c>
@@ -9013,7 +9603,6 @@
       <c r="C150" s="1" t="s">
         <v>438</v>
       </c>
-      <c r="D150" s="1"/>
       <c r="E150" s="1" t="s">
         <v>739</v>
       </c>
@@ -9041,8 +9630,11 @@
       <c r="M150" s="1">
         <v>0.33679999999999999</v>
       </c>
-    </row>
-    <row r="151" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N150" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="151" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A151" s="1">
         <v>963</v>
       </c>
@@ -9082,8 +9674,11 @@
       <c r="M151" s="1">
         <v>0.33679999999999999</v>
       </c>
-    </row>
-    <row r="152" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N151" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="152" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A152" s="1">
         <v>1194</v>
       </c>
@@ -9122,6 +9717,9 @@
       </c>
       <c r="M152" s="1">
         <v>0.20100000000000001</v>
+      </c>
+      <c r="N152" t="s">
+        <v>801</v>
       </c>
     </row>
   </sheetData>

</xml_diff>